<commit_message>
Updated tools for megSAP to the newest version (freebayes, VEP, samtools,...)
data/download_tools*: updated install instructions

doc/update_overview.xlsx: updated tools

settings.ini.default: updated tools

settings_nightly.ini: updated tools

src/NGS/an_vep.php: reactivated GeneSplicer

src/NGS/mapping_star.php: parameter change for samblaster 0.1.26

src/NGS/vcf2gsvar.php: allow empty CADD scores, fixed annotaed disease group

test/data/*: updated test data

test/data_*: updated test data
</commit_message>
<xml_diff>
--- a/doc/update_overview.xlsx
+++ b/doc/update_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="152">
   <si>
     <t>database</t>
   </si>
@@ -235,48 +235,9 @@
     <t>ClinGen</t>
   </si>
   <si>
-    <t>11.2019 (1.2.0)</t>
-  </si>
-  <si>
-    <t>11.2019 (1.9)</t>
-  </si>
-  <si>
-    <t>Version 1.3.1 hat eine Bug, daher kein Update: https://github.com/ekg/freebayes/issues/560</t>
-  </si>
-  <si>
-    <t>11.2019 (0.1.24)</t>
-  </si>
-  <si>
     <t>11.2019 (0.7.17)</t>
   </si>
   <si>
-    <t>11.2019 (1.16.2)</t>
-  </si>
-  <si>
-    <t>11.2019 (v1.0.4)</t>
-  </si>
-  <si>
-    <t>11.2019 (1.0.1)</t>
-  </si>
-  <si>
-    <t>11.2019 (2.22)</t>
-  </si>
-  <si>
-    <t>11.2019 (1.6.0)</t>
-  </si>
-  <si>
-    <t>11.2019 (2.9.10)</t>
-  </si>
-  <si>
-    <t>11.2019 (96.3)</t>
-  </si>
-  <si>
-    <t>Bug: https://github.com/obophenotype/human-phenotype-ontology/issues/4916</t>
-  </si>
-  <si>
-    <t>Version 98.3 hat mehrere Bugs, daher kein Update: https://github.com/Ensembl/ensembl-vep/issues/641</t>
-  </si>
-  <si>
     <t>ftp://ftp.ebi.ac.uk/pub/databases/genenames/</t>
   </si>
   <si>
@@ -340,12 +301,6 @@
     <t>pipeline, NGSDImportHGNC</t>
   </si>
   <si>
-    <t>04.2020 (0.2.2)</t>
-  </si>
-  <si>
-    <t>04.2020 (1.9.0)</t>
-  </si>
-  <si>
     <t>04.2020 (2.0.0)</t>
   </si>
   <si>
@@ -361,36 +316,15 @@
     <t>notes</t>
   </si>
   <si>
-    <t>05.2020 (140131)</t>
-  </si>
-  <si>
     <t>ftp://ftp.ncbi.nlm.nih.gov/pub/clinvar/vcf_GRCh37/archive_2.0/2020/</t>
   </si>
   <si>
     <t>05.2020 (20200506)</t>
   </si>
   <si>
-    <t>05.2020 (2.1.1)</t>
-  </si>
-  <si>
-    <t>05.2020 (02.2014)</t>
-  </si>
-  <si>
-    <t>05.2020 (1.6)</t>
-  </si>
-  <si>
-    <t>05.2020 (09.2014)</t>
-  </si>
-  <si>
-    <t>05.2020 (07.2017)</t>
-  </si>
-  <si>
     <t>there is a new version with additional GRCh38 coordinates</t>
   </si>
   <si>
-    <t>05.2020 (1.1)</t>
-  </si>
-  <si>
     <t>05.2020 (2020.1)</t>
   </si>
   <si>
@@ -401,13 +335,148 @@
   </si>
   <si>
     <t>07.2020 (latest - not versioned)</t>
+  </si>
+  <si>
+    <t>07.2020 (140131)</t>
+  </si>
+  <si>
+    <t>new version from July 23</t>
+  </si>
+  <si>
+    <t>07.2020 (2.1.1)</t>
+  </si>
+  <si>
+    <t>update GSvar IGV file, clinvar_20200720.vcf.gz available</t>
+  </si>
+  <si>
+    <t>07.2020 (02.2014)</t>
+  </si>
+  <si>
+    <t>07.2020 (1.6)</t>
+  </si>
+  <si>
+    <t>07.2020 (09.2014)</t>
+  </si>
+  <si>
+    <t>07.2020 (1.1)</t>
+  </si>
+  <si>
+    <t>Jul 23 2020</t>
+  </si>
+  <si>
+    <t>June Release available,    Bug: https://github.com/obophenotype/human-phenotype-ontology/issues/4916</t>
+  </si>
+  <si>
+    <t>July 2020 version available</t>
+  </si>
+  <si>
+    <t>07.2020 (1.0.1)</t>
+  </si>
+  <si>
+    <t>07.2020 (2.22)</t>
+  </si>
+  <si>
+    <t>Test https://github.com/bwa-mem2/bwa-mem2</t>
+  </si>
+  <si>
+    <t>07.2020 (1.16.6)</t>
+  </si>
+  <si>
+    <t>07.2020 (1.6.0)</t>
+  </si>
+  <si>
+    <t>07.2020 (2.9.10)</t>
+  </si>
+  <si>
+    <t>1.0.5 available</t>
+  </si>
+  <si>
+    <t>2.7.5a available</t>
+  </si>
+  <si>
+    <t>2.0.1 available</t>
+  </si>
+  <si>
+    <t>07.2020 (0.2.2)</t>
+  </si>
+  <si>
+    <t>07.2020 (1.9.0)</t>
+  </si>
+  <si>
+    <t>07.2020 (07.2017)</t>
+  </si>
+  <si>
+    <t>InterOp</t>
+  </si>
+  <si>
+    <t>Circos</t>
+  </si>
+  <si>
+    <t>ExpansionHunter</t>
+  </si>
+  <si>
+    <t>circos plot with CNVs,ROHS,…</t>
+  </si>
+  <si>
+    <t>Repeat expansion calling</t>
+  </si>
+  <si>
+    <t>07.2020 (3.22)</t>
+  </si>
+  <si>
+    <t>https://github.com/Illumina/ExpansionHunter</t>
+  </si>
+  <si>
+    <t>http://circos.ca/software/download/</t>
+  </si>
+  <si>
+    <t>07.2020 (0.69-9)</t>
+  </si>
+  <si>
+    <t>reading InterOp metric files (Illumina NextSeq 1k/2k)</t>
+  </si>
+  <si>
+    <t>07.2020 (1.0.25)</t>
+  </si>
+  <si>
+    <t>v1.1.10 available</t>
+  </si>
+  <si>
+    <t>varscan2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variant calling </t>
+  </si>
+  <si>
+    <t>07.2020 (2.4.4)</t>
+  </si>
+  <si>
+    <t>https://github.com/dkoboldt/varscan</t>
+  </si>
+  <si>
+    <t>08.2020 (1.3.2)</t>
+  </si>
+  <si>
+    <t>08.2020 (1.10)</t>
+  </si>
+  <si>
+    <t>08.2020 (0.1.26)</t>
+  </si>
+  <si>
+    <t>08.2020 (100.3)</t>
+  </si>
+  <si>
+    <t>08.2020 (v1.0.5)</t>
+  </si>
+  <si>
+    <t>Bug (fehlender CADD score): https://github.com/Ensembl/ensembl-vep/issues/812</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,6 +534,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -502,7 +577,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -558,6 +633,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -861,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,13 +970,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -905,12 +986,14 @@
       <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="14"/>
+      <c r="C2" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>108</v>
+      </c>
       <c r="E2" s="21" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,28 +1004,28 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="25" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
-        <v>117</v>
+      <c r="C4" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -953,14 +1036,14 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="25" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -971,11 +1054,11 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D6"/>
       <c r="E6" s="21" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -986,11 +1069,11 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D7"/>
       <c r="E7" s="25" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F7" s="18"/>
     </row>
@@ -1002,11 +1085,11 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D8"/>
       <c r="E8" s="25" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,15 +1099,15 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>122</v>
+      <c r="C9" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="25" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,11 +1118,11 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="25" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1050,28 +1133,28 @@
         <v>32</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="22" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1079,17 +1162,19 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>115</v>
+      </c>
       <c r="E13" s="25" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,11 +1185,11 @@
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="21" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1114,15 +1199,15 @@
       <c r="B15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
-        <v>127</v>
+      <c r="C15" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="21" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,28 +1217,31 @@
       <c r="B16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
-        <v>112</v>
+      <c r="C16" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" t="s">
-        <v>112</v>
+        <v>90</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1173,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>21</v>
@@ -1200,12 +1288,10 @@
       <c r="B22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>75</v>
-      </c>
+      <c r="C22" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="15"/>
       <c r="E22" s="12" t="s">
         <v>24</v>
       </c>
@@ -1218,8 +1304,8 @@
       <c r="B23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>74</v>
+      <c r="C23" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
@@ -1235,7 +1321,7 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12" t="s">
@@ -1250,7 +1336,7 @@
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="D25"/>
       <c r="E25" s="12" t="s">
@@ -1265,8 +1351,8 @@
       <c r="B26" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C26" t="s">
-        <v>76</v>
+      <c r="C26" s="23" t="s">
+        <v>148</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="12" t="s">
@@ -1280,10 +1366,12 @@
       <c r="B27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="10"/>
+      <c r="C27" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="E27" s="12" t="s">
         <v>22</v>
       </c>
@@ -1296,7 +1384,7 @@
         <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="12" t="s">
@@ -1311,11 +1399,11 @@
       <c r="B29" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
-        <v>84</v>
+      <c r="C29" s="23" t="s">
+        <v>149</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>54</v>
@@ -1329,240 +1417,307 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="3"/>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B35" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C35" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="9" t="s">
+      <c r="D35" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C33" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="12" t="s">
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="12" t="s">
-        <v>39</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="12" t="s">
+      <c r="C42" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B43" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C39" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="12" t="s">
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C40" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="12" t="s">
+      <c r="C44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76" s="3"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77" s="3"/>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1573,27 +1728,30 @@
     <hyperlink ref="E25" r:id="rId5"/>
     <hyperlink ref="E27" r:id="rId6"/>
     <hyperlink ref="E29" r:id="rId7"/>
-    <hyperlink ref="E33" r:id="rId8"/>
+    <hyperlink ref="E36" r:id="rId8"/>
     <hyperlink ref="E30" r:id="rId9"/>
-    <hyperlink ref="E34" r:id="rId10"/>
-    <hyperlink ref="E3" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E4" r:id="rId13"/>
-    <hyperlink ref="E5" r:id="rId14"/>
-    <hyperlink ref="E28" r:id="rId15"/>
-    <hyperlink ref="E7" r:id="rId16"/>
-    <hyperlink ref="E6" r:id="rId17" location="gerp"/>
-    <hyperlink ref="E8" r:id="rId18"/>
-    <hyperlink ref="E9" r:id="rId19"/>
-    <hyperlink ref="E10" r:id="rId20"/>
-    <hyperlink ref="E12" r:id="rId21"/>
-    <hyperlink ref="E15" r:id="rId22"/>
-    <hyperlink ref="E14" r:id="rId23"/>
-    <hyperlink ref="E11" r:id="rId24"/>
-    <hyperlink ref="E16" r:id="rId25"/>
-    <hyperlink ref="E17" r:id="rId26"/>
+    <hyperlink ref="E37" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E4" r:id="rId12"/>
+    <hyperlink ref="E5" r:id="rId13"/>
+    <hyperlink ref="E28" r:id="rId14"/>
+    <hyperlink ref="E7" r:id="rId15"/>
+    <hyperlink ref="E6" r:id="rId16" location="gerp"/>
+    <hyperlink ref="E8" r:id="rId17"/>
+    <hyperlink ref="E9" r:id="rId18"/>
+    <hyperlink ref="E10" r:id="rId19"/>
+    <hyperlink ref="E12" r:id="rId20"/>
+    <hyperlink ref="E15" r:id="rId21"/>
+    <hyperlink ref="E14" r:id="rId22"/>
+    <hyperlink ref="E11" r:id="rId23"/>
+    <hyperlink ref="E16" r:id="rId24"/>
+    <hyperlink ref="E17" r:id="rId25"/>
+    <hyperlink ref="E3" r:id="rId26"/>
+    <hyperlink ref="E41" r:id="rId27"/>
+    <hyperlink ref="E42" r:id="rId28"/>
+    <hyperlink ref="E43" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
doc/update_overview.xlsx: updated tool update overview
</commit_message>
<xml_diff>
--- a/doc/update_overview.xlsx
+++ b/doc/update_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="150">
   <si>
     <t>database</t>
   </si>
@@ -235,9 +235,6 @@
     <t>ClinGen</t>
   </si>
   <si>
-    <t>11.2019 (0.7.17)</t>
-  </si>
-  <si>
     <t>ftp://ftp.ebi.ac.uk/pub/databases/genenames/</t>
   </si>
   <si>
@@ -301,12 +298,6 @@
     <t>pipeline, NGSDImportHGNC</t>
   </si>
   <si>
-    <t>04.2020 (2.0.0)</t>
-  </si>
-  <si>
-    <t>04.2020 (2.7.3a)</t>
-  </si>
-  <si>
     <t>05.2020 (latest - not versioned)</t>
   </si>
   <si>
@@ -370,27 +361,6 @@
     <t>July 2020 version available</t>
   </si>
   <si>
-    <t>07.2020 (1.0.1)</t>
-  </si>
-  <si>
-    <t>07.2020 (2.22)</t>
-  </si>
-  <si>
-    <t>Test https://github.com/bwa-mem2/bwa-mem2</t>
-  </si>
-  <si>
-    <t>07.2020 (1.16.6)</t>
-  </si>
-  <si>
-    <t>07.2020 (1.6.0)</t>
-  </si>
-  <si>
-    <t>07.2020 (2.9.10)</t>
-  </si>
-  <si>
-    <t>1.0.5 available</t>
-  </si>
-  <si>
     <t>2.7.5a available</t>
   </si>
   <si>
@@ -421,36 +391,21 @@
     <t>Repeat expansion calling</t>
   </si>
   <si>
-    <t>07.2020 (3.22)</t>
-  </si>
-  <si>
     <t>https://github.com/Illumina/ExpansionHunter</t>
   </si>
   <si>
     <t>http://circos.ca/software/download/</t>
   </si>
   <si>
-    <t>07.2020 (0.69-9)</t>
-  </si>
-  <si>
     <t>reading InterOp metric files (Illumina NextSeq 1k/2k)</t>
   </si>
   <si>
-    <t>07.2020 (1.0.25)</t>
-  </si>
-  <si>
-    <t>v1.1.10 available</t>
-  </si>
-  <si>
     <t>varscan2</t>
   </si>
   <si>
     <t xml:space="preserve">variant calling </t>
   </si>
   <si>
-    <t>07.2020 (2.4.4)</t>
-  </si>
-  <si>
     <t>https://github.com/dkoboldt/varscan</t>
   </si>
   <si>
@@ -470,6 +425,45 @@
   </si>
   <si>
     <t>Bug (fehlender CADD score): https://github.com/Ensembl/ensembl-vep/issues/812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bwa2 available (https://github.com/bwa-mem2/bwa-mem2), but has high memory requirements. Can be used if shared memory feature is implemented (https://github.com/bwa-mem2/bwa-mem2/issues/65) </t>
+  </si>
+  <si>
+    <t>08.2020 (1.0.1)</t>
+  </si>
+  <si>
+    <t>08.2020 (2.22)</t>
+  </si>
+  <si>
+    <t>08.2020 (0.7.17)</t>
+  </si>
+  <si>
+    <t>08.2020 (1.16.6)</t>
+  </si>
+  <si>
+    <t>08.2020 (1.6.0)</t>
+  </si>
+  <si>
+    <t>08.2020 (1.0.25)</t>
+  </si>
+  <si>
+    <t>08.2020 (0.69-9)</t>
+  </si>
+  <si>
+    <t>08.2020 (3.22)</t>
+  </si>
+  <si>
+    <t>08.2020 (2.9.10)</t>
+  </si>
+  <si>
+    <t>08.2020 (2.4.4)</t>
+  </si>
+  <si>
+    <t>08.2020 (2.7.3a)</t>
+  </si>
+  <si>
+    <t>08.2020 (2.0.0)</t>
   </si>
 </sst>
 </file>
@@ -577,7 +571,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -638,6 +632,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -945,7 +942,7 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +950,7 @@
     <col min="1" max="1" width="47.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="106.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="108.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="73" style="2" customWidth="1"/>
     <col min="6" max="6" width="63.42578125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
@@ -970,13 +967,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -987,13 +984,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1004,28 +1001,28 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1036,14 +1033,14 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1054,11 +1051,11 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D6"/>
       <c r="E6" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,11 +1066,11 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D7"/>
       <c r="E7" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="18"/>
     </row>
@@ -1085,11 +1082,11 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D8"/>
       <c r="E8" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,14 +1097,14 @@
         <v>3</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,11 +1115,11 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1133,28 +1130,28 @@
         <v>32</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1162,19 +1159,19 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>97</v>
-      </c>
       <c r="D13" s="27" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,11 +1182,11 @@
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1200,14 +1197,14 @@
         <v>30</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1218,30 +1215,30 @@
         <v>31</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>90</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,7 +1258,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>21</v>
@@ -1289,7 +1286,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="12" t="s">
@@ -1305,7 +1302,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
@@ -1321,7 +1318,7 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12" t="s">
@@ -1336,7 +1333,7 @@
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="D25"/>
       <c r="E25" s="12" t="s">
@@ -1352,14 +1349,14 @@
         <v>17</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>18</v>
       </c>
@@ -1367,10 +1364,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>120</v>
+        <v>140</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>137</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>22</v>
@@ -1384,7 +1381,7 @@
         <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="12" t="s">
@@ -1400,10 +1397,10 @@
         <v>20</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>54</v>
@@ -1417,7 +1414,7 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="12" t="s">
@@ -1426,47 +1423,45 @@
     </row>
     <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>141</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="13"/>
       <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="12" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="12" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>21</v>
@@ -1503,7 +1498,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="12" t="s">
@@ -1519,11 +1514,9 @@
         <v>62</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>124</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D37" s="10"/>
       <c r="E37" s="28" t="s">
         <v>57</v>
       </c>
@@ -1531,17 +1524,17 @@
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="28" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -1563,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>21</v>
@@ -1577,10 +1570,10 @@
         <v>19</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="E41" s="28" t="s">
         <v>39</v>
@@ -1594,10 +1587,10 @@
         <v>70</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E42" s="28" t="s">
         <v>40</v>
@@ -1611,7 +1604,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="28" t="s">
@@ -1626,7 +1619,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="12" t="s">

</xml_diff>

<commit_message>
analyze_rna.php: STAR-Fusion only works with samtools 1.7 in some cases. Thus added tools samtools_star-fusion
</commit_message>
<xml_diff>
--- a/doc/update_overview.xlsx
+++ b/doc/update_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="154">
   <si>
     <t>database</t>
   </si>
@@ -467,6 +467,15 @@
   </si>
   <si>
     <t>test GATK on twin de-novo data: /mnt/share/evaluations/2020_07_29_twin_denovo/</t>
+  </si>
+  <si>
+    <t>10.2020 (1.7)</t>
+  </si>
+  <si>
+    <t>https://github.com/samtools/samtools/releases/download/1.7/samtools-1.7.tar.bz2</t>
+  </si>
+  <si>
+    <t>STAR-Fusion needs specific samtools version for certain RNA samples</t>
   </si>
 </sst>
 </file>
@@ -945,7 +954,7 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,6 +1640,23 @@
         <v>47</v>
       </c>
       <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>

</xml_diff>